<commit_message>
Fin du projet TPI
</commit_message>
<xml_diff>
--- a/doc/rapport_tests.xlsx
+++ b/doc/rapport_tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="104">
   <si>
     <t>A tester</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Supprimer l'article depuis la page article en tant qu'administrateur</t>
   </si>
   <si>
-    <t>Numéro de test</t>
-  </si>
-  <si>
     <t>T1</t>
   </si>
   <si>
@@ -287,16 +284,58 @@
     <t>T30</t>
   </si>
   <si>
-    <t>T31</t>
-  </si>
-  <si>
-    <t>T32</t>
-  </si>
-  <si>
     <t>La commande passée est ajoutée à l'historique des commandes et est accessible sur la page user.php</t>
   </si>
   <si>
     <t>Aller sur la page user.php et vérifier que la commande à bien été ajoutée à l'historique de commande</t>
+  </si>
+  <si>
+    <t>Vérifier que la commande qu'on vient d'effectuer contient bien les articles qu'on a commandé</t>
+  </si>
+  <si>
+    <t>Aller sur la page user.php et vérifier que la dernière commande contient tous les articles qu'on à ajouté</t>
+  </si>
+  <si>
+    <t>Le bouton payer la comande est désactiver si le solde du porte-monnaie est insuffisant</t>
+  </si>
+  <si>
+    <t>Ajouter des artices pour que le total de la commande dépasse le solde du porte-monnaie</t>
+  </si>
+  <si>
+    <t>Le prix d'un article ajouté dans le panier n'est pas affécté par le changement de son prix par la suite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter un article dans le panier, changé le prix de l'article avec l'administrateur et voir si le prix de l'article dans le panier a changé </t>
+  </si>
+  <si>
+    <t>Commande</t>
+  </si>
+  <si>
+    <t>La page produits.php affiche 12 articles par page</t>
+  </si>
+  <si>
+    <t>Aller sur la page produits.php et vérifier qu'il y a bien 12 articles par pages et qu'il y a des liens en bas pour naviguer entre les pages de produits</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>Vérifier que trier les articles par prix trie les prix ascendant et descendant</t>
+  </si>
+  <si>
+    <t>Cliquer sur le lien "Prix" pour trier les prix ascendant, descendant et vérifier que le prix sont bien trié</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Les articles sont bien trié par catégories </t>
+  </si>
+  <si>
+    <t>Cliquer sur le lien "Catégorie" pour trier les articles par catégorie et vérifier que les articles sont bien trié par catégorie</t>
+  </si>
+  <si>
+    <t>Filtres</t>
+  </si>
+  <si>
+    <t>N° de test</t>
   </si>
 </sst>
 </file>
@@ -345,7 +384,7 @@
       <name val="Montserrat Medium"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +394,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -543,9 +588,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -555,40 +616,49 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,14 +939,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F35"/>
+  <dimension ref="B2:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
@@ -884,9 +957,9 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" ht="37.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="21"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="6" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>0</v>
@@ -898,27 +971,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="57.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="13" t="s">
+    <row r="4" spans="2:6" ht="61.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="15"/>
+      <c r="C5" s="23" t="s">
         <v>35</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -931,26 +1004,26 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="61.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
-      <c r="C6" s="16" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="61.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="61.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>16</v>
@@ -963,24 +1036,24 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
@@ -993,26 +1066,26 @@
       </c>
     </row>
     <row r="10" spans="2:6" ht="61.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10"/>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="61.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>41</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="61.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>18</v>
@@ -1025,24 +1098,24 @@
       </c>
     </row>
     <row r="12" spans="2:6" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="16" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="81" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="23" t="s">
         <v>43</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="81" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>22</v>
@@ -1055,26 +1128,26 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="81.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="9"/>
-      <c r="C14" s="16" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="81.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="25" t="s">
         <v>45</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="81.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>26</v>
@@ -1087,24 +1160,24 @@
       </c>
     </row>
     <row r="16" spans="2:6" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="18" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="81.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="16"/>
+      <c r="C17" s="25" t="s">
         <v>47</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="81.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10"/>
-      <c r="C17" s="11" t="s">
-        <v>48</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>30</v>
@@ -1117,280 +1190,273 @@
       </c>
     </row>
     <row r="18" spans="2:6" ht="153.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="102" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="121.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="C20" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="102" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
+      <c r="E20" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="81" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="122.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="16"/>
+      <c r="C23" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="81" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="20" t="s">
+      <c r="D23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="102" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="122.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10"/>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="102" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="16" t="s">
+      <c r="E24" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="162" x14ac:dyDescent="0.25">
+      <c r="B25" s="15"/>
+      <c r="C25" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D25" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="F25" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="15"/>
+      <c r="C26" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="162.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="16"/>
+      <c r="C27" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="102" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="162.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="9"/>
-      <c r="C25" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="102" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="22"/>
-      <c r="C26" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="19" t="s">
+      <c r="E28" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E26" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="C27" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="F28" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="121.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="20"/>
+      <c r="C29" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="122.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="21"/>
+      <c r="C30" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="C28" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="162" x14ac:dyDescent="0.25">
-      <c r="C29" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="C30" s="16" t="s">
+      <c r="F30" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="163.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="162" x14ac:dyDescent="0.25">
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="122.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="C32" s="16" t="s">
+      <c r="D32" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="142.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="28"/>
+      <c r="C33" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" ht="162" x14ac:dyDescent="0.25">
-      <c r="C33" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="C34" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" ht="162" x14ac:dyDescent="0.25">
-      <c r="C35" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="D33" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B24:B25"/>
+  <mergeCells count="8">
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B32:B33"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B19:B23"/>
+    <mergeCell ref="B24:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>